<commit_message>
exp/Lots of lstm experiments
</commit_message>
<xml_diff>
--- a/models/lstm-global-univariate-tune-dataset1-200-trials/MASE metrics  global vs local dataset1.xlsx
+++ b/models/lstm-global-univariate-tune-dataset1-200-trials/MASE metrics  global vs local dataset1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\archie\code\Masteroppgave\models\lstm-global-univariate-tune-dataset1-200-trials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A13474DB-66FE-47D5-96FF-51657CC98789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B0B69E-2053-44BE-8CB4-DAD3DAD34BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38265" yWindow="1620" windowWidth="34365" windowHeight="20505" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="38265" yWindow="375" windowWidth="34365" windowHeight="20505" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="hidden" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="27">
   <si>
     <t>Global model MASE on dataset1</t>
   </si>
@@ -112,12 +112,15 @@
   </si>
   <si>
     <t>Dataset 1</t>
+  </si>
+  <si>
+    <t>Global model tune after test loop fix</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -534,7 +537,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -550,7 +553,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -565,11 +568,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,6 +932,9 @@
       <c r="B24" t="s">
         <v>19</v>
       </c>
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -938,6 +944,13 @@
         <v>4</v>
       </c>
       <c r="C25" s="6"/>
+      <c r="F25">
+        <v>1.0960000000000001</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -945,6 +958,11 @@
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
+      <c r="F26">
+        <v>0.78256000000000003</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -956,6 +974,15 @@
       <c r="C27" s="4">
         <v>1.0357084210526317</v>
       </c>
+      <c r="F27">
+        <v>1.2548600000000001</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1.440548947368421</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -967,6 +994,15 @@
       <c r="C28" s="4">
         <v>0.15137945476422904</v>
       </c>
+      <c r="F28">
+        <v>0.71653999999999995</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0.34545852209356903</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -978,6 +1014,15 @@
       <c r="C29" s="4">
         <v>0.81094999999999995</v>
       </c>
+      <c r="F29">
+        <v>1.1507000000000001</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="4">
+        <v>1.07944</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -989,6 +1034,15 @@
       <c r="C30" s="4" t="e">
         <v>#N/A</v>
       </c>
+      <c r="F30">
+        <v>0.71194000000000002</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="4" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1000,6 +1054,15 @@
       <c r="C31" s="4">
         <v>0.65984774544556124</v>
       </c>
+      <c r="F31">
+        <v>0.72307999999999995</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="4">
+        <v>1.5058187869907806</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -1011,8 +1074,17 @@
       <c r="C32" s="4">
         <v>0.43539904716959021</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>1.4930000000000001</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H32" s="4">
+        <v>2.2674902192543862</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.80779000000000001</v>
       </c>
@@ -1022,8 +1094,17 @@
       <c r="C33" s="4">
         <v>8.3923374799126833</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>1.0366</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="4">
+        <v>15.146573058098053</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.81094999999999995</v>
       </c>
@@ -1033,8 +1114,17 @@
       <c r="C34" s="4">
         <v>2.7204673375969994</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>1.67167</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="4">
+        <v>3.7517685480969303</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.55866000000000005</v>
       </c>
@@ -1044,8 +1134,17 @@
       <c r="C35" s="4">
         <v>2.7881499999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>0.5736</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="4">
+        <v>6.7971900000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1.5581499999999999</v>
       </c>
@@ -1055,8 +1154,17 @@
       <c r="C36" s="4">
         <v>0.55866000000000005</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>2.4283700000000001</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0.5736</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.95835999999999999</v>
       </c>
@@ -1066,8 +1174,17 @@
       <c r="C37" s="4">
         <v>3.3468100000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>1.50444</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="4">
+        <v>7.3707900000000004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0.81437999999999999</v>
       </c>
@@ -1077,8 +1194,17 @@
       <c r="C38" s="4">
         <v>19.678460000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F38">
+        <v>1.38266</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="4">
+        <v>27.370429999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0.55923999999999996</v>
       </c>
@@ -1088,33 +1214,57 @@
       <c r="C39" s="5">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>0.57755999999999996</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0.65847</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>0.83343</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0.95426</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>1.07944</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3.3468100000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>7.3707900000000004</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.70221</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F43">
+        <v>0.98319000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>22</v>
       </c>
@@ -1586,5 +1736,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
exp/LSTM global/local univariate experiments on new dataset1
</commit_message>
<xml_diff>
--- a/models/lstm-global-univariate-tune-dataset1-200-trials/MASE metrics  global vs local dataset1.xlsx
+++ b/models/lstm-global-univariate-tune-dataset1-200-trials/MASE metrics  global vs local dataset1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\archie\code\Masteroppgave\models\lstm-global-univariate-tune-dataset1-200-trials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B0B69E-2053-44BE-8CB4-DAD3DAD34BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3F3C03-D6C1-4FC3-BDC9-F11099E2C4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38265" yWindow="375" windowWidth="34365" windowHeight="20505" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24225" yWindow="2535" windowWidth="57600" windowHeight="15345" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="hidden" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="32">
   <si>
     <t>Global model MASE on dataset1</t>
   </si>
@@ -115,6 +115,21 @@
   </si>
   <si>
     <t>Global model tune after test loop fix</t>
+  </si>
+  <si>
+    <t>lstm-univariate-predict-dataset1-new-dataset</t>
+  </si>
+  <si>
+    <t>lstm-univariate-predict-dataset1-new-dataset-MSE-error</t>
+  </si>
+  <si>
+    <t>lstm-global-univariate-tune-500-trials-latest-dataset1</t>
+  </si>
+  <si>
+    <t>MASE_7_days</t>
+  </si>
+  <si>
+    <t>lstm-local-univariate-tune-500-trials-latest-dataset1</t>
   </si>
 </sst>
 </file>
@@ -569,10 +584,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:Y69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,12 +599,12 @@
     <col min="10" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -602,8 +617,23 @@
       <c r="J2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2.5642299999999998</v>
       </c>
@@ -618,8 +648,39 @@
         <v>4</v>
       </c>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>0.90122000000000002</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="6"/>
+      <c r="O3">
+        <v>1.28241</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="6"/>
+      <c r="S3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U3" s="6"/>
+      <c r="W3">
+        <v>1.18001</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y3" s="6"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.81964999999999999</v>
       </c>
@@ -630,8 +691,31 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <v>0.89463000000000004</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4">
+        <v>0.79078000000000004</v>
+      </c>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="S4">
+        <v>2.7536900000000002</v>
+      </c>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="W4">
+        <v>0.64185999999999999</v>
+      </c>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.81998000000000004</v>
       </c>
@@ -650,8 +734,47 @@
       <c r="J5" s="2">
         <v>1.2557549999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>0.58631</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="4">
+        <v>1.4016194736842107</v>
+      </c>
+      <c r="O5">
+        <v>0.70955000000000001</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>1.3917794736842106</v>
+      </c>
+      <c r="S5">
+        <v>0.79454999999999998</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U5" s="4">
+        <v>1.2567268421052631</v>
+      </c>
+      <c r="W5">
+        <v>0.61384000000000005</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>1.1907065000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.81496000000000002</v>
       </c>
@@ -670,8 +793,47 @@
       <c r="J6" s="2">
         <v>0.19860818658174098</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>11</v>
+      </c>
+      <c r="L6">
+        <v>3.18086</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0.21200615930376446</v>
+      </c>
+      <c r="O6">
+        <v>3.3651200000000001</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>0.17686123226101633</v>
+      </c>
+      <c r="S6">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="U6" s="4">
+        <v>0.14715910350328454</v>
+      </c>
+      <c r="W6">
+        <v>0.63936999999999999</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y6" s="4">
+        <v>0.11553752900948853</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1.0138199999999999</v>
       </c>
@@ -690,8 +852,47 @@
       <c r="J7" s="2">
         <v>0.93329499999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>13</v>
+      </c>
+      <c r="L7">
+        <v>0.51934000000000002</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="O7">
+        <v>0.48583999999999999</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>1.28241</v>
+      </c>
+      <c r="S7">
+        <v>0.62422999999999995</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="U7" s="4">
+        <v>1.1284799999999999</v>
+      </c>
+      <c r="W7">
+        <v>1.3398000000000001</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y7" s="4">
+        <v>1.1910150000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.81823000000000001</v>
       </c>
@@ -712,8 +913,47 @@
         <f>#N/A</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>20</v>
+      </c>
+      <c r="L8">
+        <v>1.09744</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O8">
+        <v>1.39544</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S8">
+        <v>1.6727000000000001</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="U8" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W8">
+        <v>0.58038000000000001</v>
+      </c>
+      <c r="X8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y8" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1.2102900000000001</v>
       </c>
@@ -732,8 +972,47 @@
       <c r="J9" s="2">
         <v>0.84262317318667268</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>22</v>
+      </c>
+      <c r="L9">
+        <v>0.68552000000000002</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0.92411342381329475</v>
+      </c>
+      <c r="O9">
+        <v>0.78176999999999996</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0.77092023845584579</v>
+      </c>
+      <c r="S9">
+        <v>0.61831000000000003</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U9" s="4">
+        <v>0.64145166079285965</v>
+      </c>
+      <c r="W9">
+        <v>0.61965999999999999</v>
+      </c>
+      <c r="X9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>0.51669953763514065</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1.49316</v>
       </c>
@@ -752,8 +1031,47 @@
       <c r="J10" s="2">
         <v>0.71001381199117741</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>24</v>
+      </c>
+      <c r="L10">
+        <v>2.5453100000000002</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0.85398562007193013</v>
+      </c>
+      <c r="O10">
+        <v>2.0245600000000001</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>0.59431801406081819</v>
+      </c>
+      <c r="S10">
+        <v>0.71479999999999999</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U10" s="4">
+        <v>0.41146023313391783</v>
+      </c>
+      <c r="W10">
+        <v>0.87441000000000002</v>
+      </c>
+      <c r="X10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y10" s="4">
+        <v>0.26697841219236812</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.93628999999999996</v>
       </c>
@@ -772,8 +1090,47 @@
       <c r="J11" s="2">
         <v>4.2064322571034367</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>26</v>
+      </c>
+      <c r="L11">
+        <v>1.2916700000000001</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0.80749955506919102</v>
+      </c>
+      <c r="O11">
+        <v>1.28596</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>0.89093012918315173</v>
+      </c>
+      <c r="S11">
+        <v>1.1284799999999999</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="U11" s="4">
+        <v>1.1063109553820039</v>
+      </c>
+      <c r="W11">
+        <v>1.7653099999999999</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y11" s="4">
+        <v>-1.0415621830145225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.92332000000000003</v>
       </c>
@@ -792,8 +1149,47 @@
       <c r="J12" s="2">
         <v>2.0133245580419956</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>27</v>
+      </c>
+      <c r="L12">
+        <v>2.2172100000000001</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="4">
+        <v>1.2759030388454851</v>
+      </c>
+      <c r="O12">
+        <v>1.7612699999999999</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>1.0970943894948855</v>
+      </c>
+      <c r="S12">
+        <v>1.3045500000000001</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="U12" s="4">
+        <v>1.2488906955797994</v>
+      </c>
+      <c r="W12">
+        <v>1.42815</v>
+      </c>
+      <c r="X12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y12" s="4">
+        <v>0.4436218081205589</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.55508000000000002</v>
       </c>
@@ -812,8 +1208,47 @@
       <c r="J13" s="2">
         <v>3.2417000000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>28</v>
+      </c>
+      <c r="L13">
+        <v>0.64158999999999999</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" s="4">
+        <v>3.1495199999999999</v>
+      </c>
+      <c r="O13">
+        <v>0.80867</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>2.8792800000000001</v>
+      </c>
+      <c r="S13">
+        <v>1.5050300000000001</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="U13" s="4">
+        <v>2.1353800000000001</v>
+      </c>
+      <c r="W13">
+        <v>1.8138799999999999</v>
+      </c>
+      <c r="X13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y13" s="4">
+        <v>1.5692300000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.5053700000000001</v>
       </c>
@@ -832,8 +1267,47 @@
       <c r="J14" s="2">
         <v>0.57196999999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>29</v>
+      </c>
+      <c r="L14">
+        <v>1.9536</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0.51934000000000002</v>
+      </c>
+      <c r="O14">
+        <v>1.9352400000000001</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>0.48583999999999999</v>
+      </c>
+      <c r="S14">
+        <v>1.5000800000000001</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="U14" s="4">
+        <v>0.61831000000000003</v>
+      </c>
+      <c r="W14">
+        <v>1.23706</v>
+      </c>
+      <c r="X14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y14" s="4">
+        <v>0.58038000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.74321000000000004</v>
       </c>
@@ -852,8 +1326,47 @@
       <c r="J15" s="2">
         <v>3.8136700000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>32</v>
+      </c>
+      <c r="L15">
+        <v>1.7427600000000001</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="4">
+        <v>3.66886</v>
+      </c>
+      <c r="O15">
+        <v>2.2582499999999999</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>3.3651200000000001</v>
+      </c>
+      <c r="S15">
+        <v>0.88714000000000004</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U15" s="4">
+        <v>2.7536900000000002</v>
+      </c>
+      <c r="W15">
+        <v>2.0217800000000001</v>
+      </c>
+      <c r="X15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y15" s="4">
+        <v>2.14961</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.97235000000000005</v>
       </c>
@@ -872,8 +1385,47 @@
       <c r="J16" s="2">
         <v>22.603589999999993</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <v>33</v>
+      </c>
+      <c r="L16">
+        <v>0.87114000000000003</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N16" s="4">
+        <v>26.630770000000002</v>
+      </c>
+      <c r="O16">
+        <v>1.0108299999999999</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>26.443810000000003</v>
+      </c>
+      <c r="S16">
+        <v>1.88357</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U16" s="4">
+        <v>23.87781</v>
+      </c>
+      <c r="W16">
+        <v>2.14961</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y16" s="4">
+        <v>23.814130000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1.5515000000000001</v>
       </c>
@@ -892,8 +1444,47 @@
       <c r="J17" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>34</v>
+      </c>
+      <c r="L17">
+        <v>0.71770999999999996</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N17" s="5">
+        <v>19</v>
+      </c>
+      <c r="O17">
+        <v>0.67940999999999996</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>19</v>
+      </c>
+      <c r="S17">
+        <v>2.6908099999999999</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U17" s="5">
+        <v>19</v>
+      </c>
+      <c r="W17">
+        <v>1.1729700000000001</v>
+      </c>
+      <c r="X17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y17" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.49009000000000003</v>
       </c>
@@ -903,29 +1494,117 @@
       <c r="J18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <v>39</v>
+      </c>
+      <c r="L18">
+        <v>1.50017</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>1.37469</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>1.1120399999999999</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0.75382000000000005</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.04254</v>
       </c>
       <c r="H19">
         <v>0.73719999999999997</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <v>41</v>
+      </c>
+      <c r="L19">
+        <v>0.63243000000000005</v>
+      </c>
+      <c r="O19">
+        <v>0.60114999999999996</v>
+      </c>
+      <c r="S19">
+        <v>0.70308000000000004</v>
+      </c>
+      <c r="W19">
+        <v>1.2020200000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2.2456399999999999</v>
       </c>
       <c r="H20">
         <v>1.2349300000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <v>51</v>
+      </c>
+      <c r="L20">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="O20">
+        <v>1.2591699999999999</v>
+      </c>
+      <c r="S20">
+        <v>1.2968500000000001</v>
+      </c>
+      <c r="W20">
+        <v>0.68167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.79117000000000004</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K21">
+        <v>54</v>
+      </c>
+      <c r="L21">
+        <v>3.66886</v>
+      </c>
+      <c r="O21">
+        <v>2.6337000000000002</v>
+      </c>
+      <c r="S21">
+        <v>0.68296000000000001</v>
+      </c>
+      <c r="W21">
+        <v>1.2184699999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S22">
+        <v>1.28894</v>
+      </c>
+      <c r="W22">
+        <v>1.8800600000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="W23" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>18</v>
       </c>
@@ -935,8 +1614,22 @@
       <c r="F24" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S24">
+        <v>4.4349999999999996</v>
+      </c>
+      <c r="T24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U24" s="6"/>
+      <c r="W24">
+        <v>1.90049</v>
+      </c>
+      <c r="X24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y24" s="6"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1.80925</v>
       </c>
@@ -951,8 +1644,18 @@
         <v>4</v>
       </c>
       <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S25">
+        <v>1.4245300000000001</v>
+      </c>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="W25">
+        <v>1.15079</v>
+      </c>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.81671000000000005</v>
       </c>
@@ -963,8 +1666,26 @@
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S26">
+        <v>0.62258999999999998</v>
+      </c>
+      <c r="T26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U26" s="4">
+        <v>1.1337925</v>
+      </c>
+      <c r="W26">
+        <v>0.53376000000000001</v>
+      </c>
+      <c r="X26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y26" s="4">
+        <v>0.99620500000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.69525000000000003</v>
       </c>
@@ -983,8 +1704,26 @@
       <c r="H27" s="4">
         <v>1.440548947368421</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S27">
+        <v>1.14655</v>
+      </c>
+      <c r="T27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="U27" s="4">
+        <v>0.18688578128713434</v>
+      </c>
+      <c r="W27">
+        <v>1.17435</v>
+      </c>
+      <c r="X27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y27" s="4">
+        <v>8.5102418075918521E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0.65658000000000005</v>
       </c>
@@ -1003,8 +1742,26 @@
       <c r="H28" s="4">
         <v>0.34545852209356903</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S28">
+        <v>0.58260000000000001</v>
+      </c>
+      <c r="T28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="U28" s="4">
+        <v>0.90684999999999993</v>
+      </c>
+      <c r="W28">
+        <v>0.46665000000000001</v>
+      </c>
+      <c r="X28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y28" s="4">
+        <v>0.99975999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0.70533000000000001</v>
       </c>
@@ -1023,8 +1780,26 @@
       <c r="H29" s="4">
         <v>1.07944</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S29">
+        <v>1.1085400000000001</v>
+      </c>
+      <c r="T29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="U29" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W29">
+        <v>1.04053</v>
+      </c>
+      <c r="X29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y29" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.79679999999999995</v>
       </c>
@@ -1043,8 +1818,26 @@
       <c r="H30" s="4" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S30">
+        <v>0.64056000000000002</v>
+      </c>
+      <c r="T30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U30" s="4">
+        <v>0.83577862197238117</v>
+      </c>
+      <c r="W30">
+        <v>0.55530000000000002</v>
+      </c>
+      <c r="X30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y30" s="4">
+        <v>0.38058958373472135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.91879</v>
       </c>
@@ -1063,8 +1856,26 @@
       <c r="H31" s="4">
         <v>1.5058187869907806</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S31">
+        <v>1.40907</v>
+      </c>
+      <c r="T31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U31" s="4">
+        <v>0.69852590494605238</v>
+      </c>
+      <c r="W31">
+        <v>1.0918399999999999</v>
+      </c>
+      <c r="X31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y31" s="4">
+        <v>0.14484843124736849</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1.55047</v>
       </c>
@@ -1083,8 +1894,26 @@
       <c r="H32" s="4">
         <v>2.2674902192543862</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="S32">
+        <v>1.18316</v>
+      </c>
+      <c r="T32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="U32" s="4">
+        <v>14.124833566915946</v>
+      </c>
+      <c r="W32">
+        <v>1.6010500000000001</v>
+      </c>
+      <c r="X32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y32" s="4">
+        <v>0.17591067052054976</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.80779000000000001</v>
       </c>
@@ -1103,8 +1932,26 @@
       <c r="H33" s="4">
         <v>15.146573058098053</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="S33">
+        <v>0.58250999999999997</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="U33" s="4">
+        <v>3.5120750838546049</v>
+      </c>
+      <c r="W33">
+        <v>0.55276000000000003</v>
+      </c>
+      <c r="X33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y33" s="4">
+        <v>0.63017266390453053</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.81094999999999995</v>
       </c>
@@ -1123,8 +1970,26 @@
       <c r="H34" s="4">
         <v>3.7517685480969303</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="S34">
+        <v>0.54198000000000002</v>
+      </c>
+      <c r="T34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="U34" s="4">
+        <v>3.8930199999999995</v>
+      </c>
+      <c r="W34">
+        <v>0.65536000000000005</v>
+      </c>
+      <c r="X34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y34" s="4">
+        <v>1.43384</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.55866000000000005</v>
       </c>
@@ -1143,8 +2008,26 @@
       <c r="H35" s="4">
         <v>6.7971900000000005</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="S35">
+        <v>0.88114999999999999</v>
+      </c>
+      <c r="T35" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="U35" s="4">
+        <v>0.54198000000000002</v>
+      </c>
+      <c r="W35">
+        <v>1.2286999999999999</v>
+      </c>
+      <c r="X35" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y35" s="4">
+        <v>0.46665000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1.5581499999999999</v>
       </c>
@@ -1163,8 +2046,26 @@
       <c r="H36" s="4">
         <v>0.5736</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="S36">
+        <v>1.15832</v>
+      </c>
+      <c r="T36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U36" s="4">
+        <v>4.4349999999999996</v>
+      </c>
+      <c r="W36">
+        <v>1.2433099999999999</v>
+      </c>
+      <c r="X36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y36" s="4">
+        <v>1.90049</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.95835999999999999</v>
       </c>
@@ -1183,8 +2084,26 @@
       <c r="H37" s="4">
         <v>7.3707900000000004</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="S37">
+        <v>1.3755500000000001</v>
+      </c>
+      <c r="T37" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U37" s="4">
+        <v>22.675850000000001</v>
+      </c>
+      <c r="W37">
+        <v>1.0988899999999999</v>
+      </c>
+      <c r="X37" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y37" s="4">
+        <v>19.924099999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>0.81437999999999999</v>
       </c>
@@ -1203,8 +2122,26 @@
       <c r="H38" s="4">
         <v>27.370429999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S38">
+        <v>0.90917000000000003</v>
+      </c>
+      <c r="T38" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U38" s="5">
+        <v>20</v>
+      </c>
+      <c r="W38">
+        <v>0.95899000000000001</v>
+      </c>
+      <c r="X38" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y38" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0.55923999999999996</v>
       </c>
@@ -1223,8 +2160,20 @@
       <c r="H39" s="5">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="S39">
+        <v>0.64348000000000005</v>
+      </c>
+      <c r="U39">
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <v>0.68991999999999998</v>
+      </c>
+      <c r="Y39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0.65847</v>
       </c>
@@ -1234,37 +2183,61 @@
       <c r="H40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="S40">
+        <v>0.90452999999999995</v>
+      </c>
+      <c r="W40">
+        <v>0.83838999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0.95426</v>
       </c>
       <c r="F41">
         <v>1.07944</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="S41">
+        <v>1.45445</v>
+      </c>
+      <c r="W41">
+        <v>1.4517</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3.3468100000000001</v>
       </c>
       <c r="F42">
         <v>7.3707900000000004</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="S42">
+        <v>0.86333000000000004</v>
+      </c>
+      <c r="W42">
+        <v>0.81611999999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.70221</v>
       </c>
       <c r="F43">
         <v>0.98319000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="S43">
+        <v>0.80878000000000005</v>
+      </c>
+      <c r="W43">
+        <v>0.87519999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>22</v>
       </c>

</xml_diff>